<commit_message>
Added Code as per the changes in studio
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/smokeTestInput.xlsx
+++ b/TestingFramework/TestData/smokeTestInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="17085" windowHeight="6000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="17085" windowHeight="5820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="12" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="bulkpro" sheetId="18" r:id="rId3"/>
     <sheet name="dashboard" sheetId="19" r:id="rId4"/>
     <sheet name="Entity" sheetId="20" r:id="rId5"/>
+    <sheet name="studiologin" sheetId="21" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="22" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="100">
   <si>
     <t>Yes</t>
   </si>
@@ -303,6 +305,21 @@
   </si>
   <si>
     <t>Save immigrationInfo</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>drivingLicenseDetailss</t>
+  </si>
+  <si>
+    <t>immigrationInfos</t>
   </si>
 </sst>
 </file>
@@ -346,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +400,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -412,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -427,6 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,10 +831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +867,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -879,7 +903,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -894,7 +918,7 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,7 +933,7 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -926,7 +950,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -941,83 +965,6 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1029,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1060,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,8 +1170,8 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>9</v>
+      <c r="B2" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>10</v>
@@ -1320,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>10</v>
@@ -1441,4 +1388,260 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Edit Component test Suite along with the report
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/smokeTestInput.xlsx
+++ b/TestingFramework/TestData/smokeTestInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="15315" windowHeight="4155" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="15315" windowHeight="4155" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="12" r:id="rId1"/>
@@ -379,7 +379,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: EditModule</t>
+      <t>: EditedModule</t>
     </r>
   </si>
   <si>
@@ -395,7 +395,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: EditSubmodule</t>
+      <t>: EditedSubmodule1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> subMod2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : EditedSubmodule2</t>
     </r>
   </si>
 </sst>
@@ -1229,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,7 +1265,7 @@
     <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="55.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="56" style="2" customWidth="1"/>
-    <col min="11" max="11" width="59.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="56" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1991,15 +2012,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Updated xpaths of project, module, submodule & process verb Added Create > View verb test code combination
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/smokeTestInput.xlsx
+++ b/TestingFramework/TestData/smokeTestInput.xlsx
@@ -4,25 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="15315" windowHeight="4155" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="15315" windowHeight="4155" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="12" r:id="rId1"/>
     <sheet name="dashboard" sheetId="22" r:id="rId2"/>
     <sheet name="studiologin" sheetId="20" r:id="rId3"/>
     <sheet name="Entity" sheetId="18" r:id="rId4"/>
-    <sheet name="MasterData" sheetId="23" r:id="rId5"/>
-    <sheet name="ProcessAndPolicies" sheetId="11" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="24" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="25" r:id="rId8"/>
-    <sheet name="Edit" sheetId="26" r:id="rId9"/>
+    <sheet name="Edit" sheetId="26" r:id="rId5"/>
+    <sheet name="MasterData" sheetId="23" r:id="rId6"/>
+    <sheet name="ProcessAndPolicies" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="24" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="25" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="27" r:id="rId10"/>
+    <sheet name="Email" sheetId="28" r:id="rId11"/>
+    <sheet name="Calender" sheetId="29" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="122">
   <si>
     <t>Yes</t>
   </si>
@@ -340,15 +343,7 @@
     <t>all</t>
   </si>
   <si>
-    <t>DrivingLicenseDetails.employeeNo,not equals,KGM921 and
-DrivingLicenseDetails.employeeNo,not equals,KGM922</t>
-  </si>
-  <si>
     <t>Business Validation</t>
-  </si>
-  <si>
-    <t>DrivingLicenseDetails.employeeNo,not equals,KGM1121 and
-DrivingLicenseDetails.employeeNo,not equals,KGM952</t>
   </si>
   <si>
     <r>
@@ -419,12 +414,58 @@
       <t xml:space="preserve"> : EditedSubmodule2</t>
     </r>
   </si>
+  <si>
+    <t>DrivingLicenseDetails.employeeNo,not equals,KGM12270 and
+DrivingLicenseDetails.employeeNo,not equals,KGM12219</t>
+  </si>
+  <si>
+    <t>DrivingLicenseDetails.employeeNo,not equals,KGM1111 and
+DrivingLicenseDetails.employeeNo,not equals,KGM1112</t>
+  </si>
+  <si>
+    <t>DrivingLicenseDetails.employeeNo,not equals,KGM9111 and
+DrivingLicenseDetails.employeeNo,not equals,KGM9112</t>
+  </si>
+  <si>
+    <t>DrivingLicenseDetails.employeeNo,not equals,KGM0191 and
+DrivingLicenseDetails.employeeNo,not equals,KGM0192</t>
+  </si>
+  <si>
+    <t>soruceType</t>
+  </si>
+  <si>
+    <t>dataForSelectedSource</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>rajamani.p@kagamierp.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>30/12/2016and30/01/2017</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +512,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -554,11 +603,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -590,8 +640,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
@@ -961,12 +1014,318 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="55.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="56" style="2" customWidth="1"/>
+    <col min="11" max="11" width="56" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1412,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,6 +1564,219 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56" style="2" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1246,12 +1818,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1895,7 @@
         <v>91</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1354,10 +1926,10 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1378,12 +1950,12 @@
         <v>103</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="16" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1440,7 +2012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -1796,7 +2368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -2006,217 +2578,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="56" style="2" customWidth="1"/>
-    <col min="9" max="9" width="59.85546875" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>